<commit_message>
a lot of succes from sky 🌹
</commit_message>
<xml_diff>
--- a/server/סימולטור פרישה - אפיון מעודכן (1).xlsx
+++ b/server/סימולטור פרישה - אפיון מעודכן (1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\יומטוביאן מרים\source\repos\RetirementSimulator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\שרגא יהודית\Downloads\RetirementSimulato\RetirementSimulator-master\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A9794B-19F3-4CD7-99D8-A39AD0831AAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B359A3-311E-48F4-8D91-ED166801C057}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9420" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12255" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="מסך 1" sheetId="1" r:id="rId1"/>
@@ -254,7 +254,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1722" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="607">
   <si>
     <t>במסך זה המשמתמש יצטרך רק לבחור אם העובד פורש בפנסיה תקציבית או בפנסיה צוברת</t>
   </si>
@@ -2375,7 +2375,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2439,6 +2439,12 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -2488,7 +2494,7 @@
     <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2704,17 +2710,18 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="4" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="1" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="2" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="1" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="2" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="4" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2727,6 +2734,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCCCC"/>
+      <color rgb="FFFF9999"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3085,7 +3098,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3104,15 +3117,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="117" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="115"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
       <c r="J2" s="88"/>
     </row>
     <row r="3" spans="2:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -4014,7 +4027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:H53"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView rightToLeft="1" topLeftCell="A37" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -4724,7 +4737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B3:L19"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
+    <sheetView rightToLeft="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -4995,8 +5008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:O411"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5030,24 +5043,24 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="117" t="s">
+      <c r="B6" s="115" t="s">
         <v>163</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="F6" s="118" t="s">
+      <c r="F6" s="119" t="s">
         <v>606</v>
       </c>
-      <c r="G6" s="118"/>
-      <c r="H6" s="118"/>
-      <c r="I6" s="118"/>
-      <c r="J6" s="118"/>
-      <c r="K6" s="118"/>
-      <c r="L6" s="118"/>
+      <c r="G6" s="119"/>
+      <c r="H6" s="119"/>
+      <c r="I6" s="119"/>
+      <c r="J6" s="119"/>
+      <c r="K6" s="119"/>
+      <c r="L6" s="119"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="117" t="s">
+      <c r="B7" s="115" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -5055,7 +5068,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="117" t="s">
+      <c r="B8" s="115" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -5063,7 +5076,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="117" t="s">
+      <c r="B9" s="115" t="s">
         <v>75</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -5071,7 +5084,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="117" t="s">
+      <c r="B10" s="115" t="s">
         <v>80</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -5079,7 +5092,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="117" t="s">
+      <c r="B11" s="115" t="s">
         <v>77</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -5087,7 +5100,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="119" t="s">
+      <c r="B12" s="116" t="s">
         <v>168</v>
       </c>
       <c r="C12" s="113" t="s">
@@ -5095,7 +5108,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="117" t="s">
+      <c r="B13" s="115" t="s">
         <v>553</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -5103,7 +5116,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="117" t="s">
+      <c r="B14" s="115" t="s">
         <v>81</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -5111,7 +5124,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="119" t="s">
+      <c r="B15" s="116" t="s">
         <v>170</v>
       </c>
       <c r="C15" s="113" t="s">
@@ -5119,7 +5132,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="117" t="s">
+      <c r="B16" s="115" t="s">
         <v>172</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -5127,7 +5140,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="117" t="s">
+      <c r="B17" s="115" t="s">
         <v>174</v>
       </c>
       <c r="C17" s="6" t="s">
@@ -5135,7 +5148,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="117" t="s">
+      <c r="B18" s="115" t="s">
         <v>118</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -5143,7 +5156,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="117" t="s">
+      <c r="B19" s="115" t="s">
         <v>137</v>
       </c>
       <c r="C19" s="6" t="s">
@@ -5152,7 +5165,7 @@
     </row>
     <row r="20" spans="1:8" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="117" t="s">
+      <c r="B21" s="115" t="s">
         <v>184</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -5160,7 +5173,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="117" t="s">
+      <c r="B22" s="115" t="s">
         <v>532</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -5174,7 +5187,7 @@
       <c r="H22" s="96"/>
     </row>
     <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B23" s="119" t="s">
+      <c r="B23" s="116" t="s">
         <v>534</v>
       </c>
       <c r="C23" s="114" t="s">
@@ -5189,7 +5202,7 @@
       <c r="H23" s="96"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="117" t="s">
+      <c r="B24" s="115" t="s">
         <v>182</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -5197,7 +5210,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="117" t="s">
+      <c r="B25" s="115" t="s">
         <v>183</v>
       </c>
       <c r="C25" s="6" t="s">
@@ -5383,7 +5396,7 @@
       <c r="F39" s="29"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B40" s="119" t="s">
+      <c r="B40" s="116" t="s">
         <v>92</v>
       </c>
       <c r="D40" s="29"/>
@@ -5393,7 +5406,7 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="119" t="s">
+      <c r="B41" s="116" t="s">
         <v>94</v>
       </c>
       <c r="D41" s="29"/>
@@ -5403,7 +5416,7 @@
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="119" t="s">
+      <c r="B42" s="116" t="s">
         <v>96</v>
       </c>
       <c r="D42" s="29"/>
@@ -5413,7 +5426,7 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="119" t="s">
+      <c r="B43" s="116" t="s">
         <v>97</v>
       </c>
       <c r="F43" s="34">
@@ -5422,7 +5435,7 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="119" t="s">
+      <c r="B44" s="116" t="s">
         <v>99</v>
       </c>
       <c r="F44" s="30">
@@ -5442,7 +5455,7 @@
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="113" t="s">
+      <c r="B47" s="116" t="s">
         <v>107</v>
       </c>
       <c r="C47" s="92" t="s">
@@ -5465,7 +5478,7 @@
       <c r="O47" s="96"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B48" s="113" t="s">
+      <c r="B48" s="116" t="s">
         <v>177</v>
       </c>
       <c r="C48" s="6" t="s">
@@ -5476,7 +5489,7 @@
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="113" t="s">
+      <c r="B49" s="120" t="s">
         <v>99</v>
       </c>
       <c r="C49" s="6" t="s">
@@ -6324,7 +6337,7 @@
       <c r="B137" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C137" s="116" t="s">
+      <c r="C137" s="118" t="s">
         <v>549</v>
       </c>
     </row>
@@ -6332,13 +6345,13 @@
       <c r="B138" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C138" s="116"/>
+      <c r="C138" s="118"/>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B139" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C139" s="116"/>
+      <c r="C139" s="118"/>
       <c r="D139" s="101">
         <v>45008</v>
       </c>
@@ -6347,31 +6360,31 @@
       <c r="B140" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C140" s="116"/>
+      <c r="C140" s="118"/>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B141" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C141" s="116"/>
+      <c r="C141" s="118"/>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B142" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C142" s="116"/>
+      <c r="C142" s="118"/>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B143" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C143" s="116"/>
+      <c r="C143" s="118"/>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B144" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C144" s="116"/>
+      <c r="C144" s="118"/>
     </row>
     <row r="146" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B146" s="56" t="s">

</xml_diff>